<commit_message>
fix pesky date lag
some clusters were sampled across 2 clusters (eg jan 25 to dec 15) took care of assigning month by majority days
</commit_message>
<xml_diff>
--- a/internal_datamap_files/DECODER_covariate_map.xlsx
+++ b/internal_datamap_files/DECODER_covariate_map.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78FA765-C168-9A46-8C37-F9E10F5A1BF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="37180" windowHeight="25020"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="25080" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
     <sheet name="old covars" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="164">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -411,9 +412,6 @@
     <t>wlthrcde_combscor_cont</t>
   </si>
   <si>
-    <t>collinear</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -517,12 +515,21 @@
   </si>
   <si>
     <t>spatial_predictions</t>
+  </si>
+  <si>
+    <t>colllinear_level</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -563,7 +570,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +611,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF544D"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -662,7 +675,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -680,6 +693,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -688,6 +703,12 @@
   </cellStyles>
   <dxfs count="31">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -701,12 +722,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1366,6 +1383,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF544D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1378,51 +1400,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AG76" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:AG76">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="cluster"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AG76" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A1:AG76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:AG79">
     <sortCondition ref="C1:C79"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="column_name"/>
-    <tableColumn id="2" name="var_label"/>
-    <tableColumn id="3" name="level"/>
-    <tableColumn id="4" name="type" dataDxfId="29"/>
-    <tableColumn id="6" name="collinear" dataDxfId="28"/>
-    <tableColumn id="9" name="risk_factor_raw" dataDxfId="27"/>
-    <tableColumn id="5" name="risk_factor_model" dataDxfId="26"/>
-    <tableColumn id="7" name="spatial_predictions" dataDxfId="25"/>
-    <tableColumn id="8" name="Column2" dataDxfId="24"/>
-    <tableColumn id="10" name="Column3" dataDxfId="23"/>
-    <tableColumn id="11" name="Column4" dataDxfId="22"/>
-    <tableColumn id="12" name="Column5" dataDxfId="21"/>
-    <tableColumn id="13" name="Column6" dataDxfId="20"/>
-    <tableColumn id="14" name="Column7" dataDxfId="19"/>
-    <tableColumn id="15" name="Column8" dataDxfId="18"/>
-    <tableColumn id="16" name="Column9" dataDxfId="17"/>
-    <tableColumn id="17" name="Column10" dataDxfId="16"/>
-    <tableColumn id="18" name="Column11" dataDxfId="15"/>
-    <tableColumn id="19" name="Column12" dataDxfId="14"/>
-    <tableColumn id="20" name="Column13" dataDxfId="13"/>
-    <tableColumn id="21" name="Column14" dataDxfId="12"/>
-    <tableColumn id="22" name="Column15" dataDxfId="11"/>
-    <tableColumn id="23" name="Column16" dataDxfId="10"/>
-    <tableColumn id="24" name="Column17" dataDxfId="9"/>
-    <tableColumn id="25" name="Column18" dataDxfId="8"/>
-    <tableColumn id="26" name="Column19" dataDxfId="7"/>
-    <tableColumn id="27" name="Column20" dataDxfId="6"/>
-    <tableColumn id="28" name="Column21" dataDxfId="5"/>
-    <tableColumn id="29" name="Column22" dataDxfId="4"/>
-    <tableColumn id="30" name="Column23" dataDxfId="3"/>
-    <tableColumn id="31" name="Column24" dataDxfId="2"/>
-    <tableColumn id="32" name="Column25" dataDxfId="1"/>
-    <tableColumn id="33" name="Column26" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="var_label"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="type" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="risk_factor_raw" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="risk_factor_model" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{86F0AA62-B09A-5A46-BD3F-BF2E1ECE7318}" name="colllinear_level" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="spatial_predictions" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column2" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column3" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column4" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column5" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column6" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column7" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column8" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column9" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column10" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column11" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column12" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column13" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column14" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column15" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column16" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column17" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column18" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column19" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column20" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Column21" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Column22" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Column23" dataDxfId="4"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Column24" dataDxfId="3"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Column25" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Column26" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1724,19 +1740,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1751,97 +1768,97 @@
         <v>85</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
@@ -1854,7 +1871,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -1897,7 +1914,7 @@
       <c r="AU2" s="6"/>
       <c r="AV2" s="6"/>
     </row>
-    <row r="3" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -1953,7 +1970,7 @@
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
     </row>
-    <row r="4" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>52</v>
       </c>
@@ -2009,7 +2026,7 @@
       <c r="AU4" s="6"/>
       <c r="AV4" s="6"/>
     </row>
-    <row r="5" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -2065,7 +2082,7 @@
       <c r="AU5" s="6"/>
       <c r="AV5" s="6"/>
     </row>
-    <row r="6" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -2121,7 +2138,7 @@
       <c r="AU6" s="6"/>
       <c r="AV6" s="6"/>
     </row>
-    <row r="7" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -2177,7 +2194,7 @@
       <c r="AU7" s="6"/>
       <c r="AV7" s="6"/>
     </row>
-    <row r="8" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
@@ -2233,7 +2250,7 @@
       <c r="AU8" s="6"/>
       <c r="AV8" s="6"/>
     </row>
-    <row r="9" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
@@ -2289,46 +2306,48 @@
       <c r="AU9" s="6"/>
       <c r="AV9" s="6"/>
     </row>
-    <row r="10" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AJ10" s="6"/>
@@ -2526,7 +2545,9 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H14" s="9" t="s">
         <v>113</v>
       </c>
@@ -2584,7 +2605,9 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H15" s="9" t="s">
         <v>113</v>
       </c>
@@ -2642,7 +2665,9 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H16" s="9" t="s">
         <v>113</v>
       </c>
@@ -2700,7 +2725,9 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H17" s="9" t="s">
         <v>113</v>
       </c>
@@ -2758,7 +2785,9 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H18" s="9" t="s">
         <v>113</v>
       </c>
@@ -2926,10 +2955,10 @@
         <v>99</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2984,10 +3013,10 @@
         <v>99</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -3043,9 +3072,11 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G23" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>113</v>
@@ -3103,9 +3134,11 @@
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G24" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>113</v>
@@ -3162,10 +3195,10 @@
         <v>99</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E25" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -3221,9 +3254,11 @@
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G26" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>113</v>
@@ -3280,10 +3315,10 @@
         <v>99</v>
       </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E27" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -3339,9 +3374,11 @@
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G28" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>113</v>
@@ -3398,12 +3435,14 @@
         <v>99</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="E29" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="F29" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>113</v>
@@ -3460,10 +3499,10 @@
         <v>99</v>
       </c>
       <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E30" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -3519,9 +3558,11 @@
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G31" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>113</v>
@@ -3578,10 +3619,10 @@
         <v>99</v>
       </c>
       <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E32" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -3627,19 +3668,19 @@
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E33" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -3685,19 +3726,19 @@
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E34" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -3753,9 +3794,11 @@
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G35" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>113</v>
@@ -3803,19 +3846,21 @@
     </row>
     <row r="36" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G36" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>113</v>
@@ -3863,19 +3908,21 @@
     </row>
     <row r="37" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
+      <c r="F37" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G37" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>113</v>
@@ -3932,10 +3979,10 @@
         <v>99</v>
       </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E38" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -3991,9 +4038,11 @@
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="G39" s="9" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>113</v>
@@ -4050,10 +4099,10 @@
         <v>99</v>
       </c>
       <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E40" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -4108,10 +4157,10 @@
         <v>99</v>
       </c>
       <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="E41" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -4167,10 +4216,10 @@
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="F42" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
@@ -4225,10 +4274,10 @@
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="F43" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -4271,7 +4320,7 @@
       <c r="AU43" s="2"/>
       <c r="AV43" s="2"/>
     </row>
-    <row r="44" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>9</v>
       </c>
@@ -4282,13 +4331,13 @@
         <v>86</v>
       </c>
       <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F44" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -4331,7 +4380,7 @@
       <c r="AU44" s="2"/>
       <c r="AV44" s="2"/>
     </row>
-    <row r="45" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>10</v>
       </c>
@@ -4342,13 +4391,13 @@
         <v>86</v>
       </c>
       <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="E45" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F45" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G45" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
@@ -4391,7 +4440,7 @@
       <c r="AU45" s="2"/>
       <c r="AV45" s="2"/>
     </row>
-    <row r="46" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>11</v>
       </c>
@@ -4447,7 +4496,7 @@
       <c r="AU46" s="2"/>
       <c r="AV46" s="2"/>
     </row>
-    <row r="47" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>14</v>
       </c>
@@ -4458,12 +4507,14 @@
         <v>86</v>
       </c>
       <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F47" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
@@ -4507,7 +4558,7 @@
       <c r="AU47" s="2"/>
       <c r="AV47" s="2"/>
     </row>
-    <row r="48" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
@@ -4518,10 +4569,10 @@
         <v>86</v>
       </c>
       <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="E48" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
@@ -4565,7 +4616,7 @@
       <c r="AU48" s="2"/>
       <c r="AV48" s="2"/>
     </row>
-    <row r="49" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>16</v>
       </c>
@@ -4577,9 +4628,11 @@
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
+      <c r="F49" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="G49" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
@@ -4623,7 +4676,7 @@
       <c r="AU49" s="2"/>
       <c r="AV49" s="2"/>
     </row>
-    <row r="50" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>17</v>
       </c>
@@ -4634,12 +4687,14 @@
         <v>86</v>
       </c>
       <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="E50" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F50" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
@@ -4683,7 +4738,7 @@
       <c r="AU50" s="2"/>
       <c r="AV50" s="2"/>
     </row>
-    <row r="51" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>18</v>
       </c>
@@ -4694,12 +4749,14 @@
         <v>86</v>
       </c>
       <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F51" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
@@ -4743,7 +4800,7 @@
       <c r="AU51" s="2"/>
       <c r="AV51" s="2"/>
     </row>
-    <row r="52" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>19</v>
       </c>
@@ -4799,7 +4856,7 @@
       <c r="AU52" s="2"/>
       <c r="AV52" s="2"/>
     </row>
-    <row r="53" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>20</v>
       </c>
@@ -4810,12 +4867,14 @@
         <v>86</v>
       </c>
       <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F53" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
@@ -4859,7 +4918,7 @@
       <c r="AU53" s="2"/>
       <c r="AV53" s="2"/>
     </row>
-    <row r="54" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>125</v>
       </c>
@@ -4870,12 +4929,14 @@
         <v>86</v>
       </c>
       <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F54" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
@@ -4919,9 +4980,9 @@
       <c r="AU54" s="2"/>
       <c r="AV54" s="2"/>
     </row>
-    <row r="55" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>79</v>
@@ -4930,12 +4991,14 @@
         <v>86</v>
       </c>
       <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="E55" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F55" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
@@ -4979,7 +5042,7 @@
       <c r="AU55" s="2"/>
       <c r="AV55" s="2"/>
     </row>
-    <row r="56" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>21</v>
       </c>
@@ -4990,12 +5053,14 @@
         <v>86</v>
       </c>
       <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="E56" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F56" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
@@ -5039,7 +5104,7 @@
       <c r="AU56" s="2"/>
       <c r="AV56" s="2"/>
     </row>
-    <row r="57" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>22</v>
       </c>
@@ -5050,10 +5115,10 @@
         <v>86</v>
       </c>
       <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="E57" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
@@ -5097,7 +5162,7 @@
       <c r="AU57" s="2"/>
       <c r="AV57" s="2"/>
     </row>
-    <row r="58" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>23</v>
       </c>
@@ -5109,9 +5174,11 @@
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+      <c r="F58" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="G58" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
@@ -5155,7 +5222,7 @@
       <c r="AU58" s="2"/>
       <c r="AV58" s="2"/>
     </row>
-    <row r="59" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>24</v>
       </c>
@@ -5166,10 +5233,10 @@
         <v>86</v>
       </c>
       <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8" t="s">
-        <v>113</v>
-      </c>
+      <c r="E59" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
@@ -5213,7 +5280,7 @@
       <c r="AU59" s="2"/>
       <c r="AV59" s="2"/>
     </row>
-    <row r="60" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>25</v>
       </c>
@@ -5225,9 +5292,11 @@
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
+      <c r="F60" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="G60" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
@@ -5271,7 +5340,7 @@
       <c r="AU60" s="2"/>
       <c r="AV60" s="2"/>
     </row>
-    <row r="61" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>26</v>
       </c>
@@ -5282,12 +5351,14 @@
         <v>86</v>
       </c>
       <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="E61" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="F61" s="8" t="s">
         <v>113</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
@@ -5331,7 +5402,7 @@
       <c r="AU61" s="2"/>
       <c r="AV61" s="2"/>
     </row>
-    <row r="62" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>59</v>
       </c>
@@ -5387,7 +5458,7 @@
       <c r="AU62" s="2"/>
       <c r="AV62" s="2"/>
     </row>
-    <row r="63" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>60</v>
       </c>
@@ -5443,7 +5514,7 @@
       <c r="AU63" s="2"/>
       <c r="AV63" s="2"/>
     </row>
-    <row r="64" spans="1:48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>61</v>
       </c>
@@ -5499,7 +5570,7 @@
       <c r="AU64" s="4"/>
       <c r="AV64" s="4"/>
     </row>
-    <row r="65" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>62</v>
       </c>
@@ -5555,7 +5626,7 @@
       <c r="AU65" s="4"/>
       <c r="AV65" s="4"/>
     </row>
-    <row r="66" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>0</v>
       </c>
@@ -5563,7 +5634,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
@@ -5611,7 +5682,7 @@
       <c r="AU66" s="4"/>
       <c r="AV66" s="4"/>
     </row>
-    <row r="67" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>1</v>
       </c>
@@ -5619,7 +5690,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
@@ -5667,7 +5738,7 @@
       <c r="AU67" s="4"/>
       <c r="AV67" s="4"/>
     </row>
-    <row r="68" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>2</v>
       </c>
@@ -5675,7 +5746,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
@@ -5723,7 +5794,7 @@
       <c r="AU68" s="4"/>
       <c r="AV68" s="4"/>
     </row>
-    <row r="69" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>3</v>
       </c>
@@ -5731,7 +5802,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
@@ -5779,7 +5850,7 @@
       <c r="AU69" s="4"/>
       <c r="AV69" s="4"/>
     </row>
-    <row r="70" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>4</v>
       </c>
@@ -5787,7 +5858,7 @@
         <v>65</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
@@ -5835,7 +5906,7 @@
       <c r="AU70" s="4"/>
       <c r="AV70" s="4"/>
     </row>
-    <row r="71" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
         <v>5</v>
       </c>
@@ -5843,7 +5914,7 @@
         <v>65</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
@@ -5891,7 +5962,7 @@
       <c r="AU71" s="4"/>
       <c r="AV71" s="4"/>
     </row>
-    <row r="72" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
         <v>6</v>
       </c>
@@ -5899,7 +5970,7 @@
         <v>67</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
@@ -5947,7 +6018,7 @@
       <c r="AU72" s="4"/>
       <c r="AV72" s="4"/>
     </row>
-    <row r="73" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>7</v>
       </c>
@@ -5955,7 +6026,7 @@
         <v>67</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
@@ -6022,7 +6093,7 @@
       <c r="BN73" s="5"/>
       <c r="BO73" s="5"/>
     </row>
-    <row r="74" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>8</v>
       </c>
@@ -6030,7 +6101,7 @@
         <v>67</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
@@ -6097,7 +6168,7 @@
       <c r="BN74" s="5"/>
       <c r="BO74" s="5"/>
     </row>
-    <row r="75" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>12</v>
       </c>
@@ -6105,7 +6176,7 @@
         <v>71</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
@@ -6172,7 +6243,7 @@
       <c r="BN75" s="5"/>
       <c r="BO75" s="5"/>
     </row>
-    <row r="76" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
         <v>13</v>
       </c>
@@ -6180,12 +6251,12 @@
         <v>72</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
+      <c r="G76" s="16"/>
       <c r="H76" s="16"/>
       <c r="I76" s="16"/>
       <c r="J76" s="16"/>
@@ -6256,7 +6327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>